<commit_message>
before install wano with hash
</commit_message>
<xml_diff>
--- a/UPDATED USER.xlsx
+++ b/UPDATED USER.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WAMii\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="WAMI ADMIN" sheetId="1" r:id="rId1"/>
     <sheet name="WAMI SALESMAN" sheetId="3" r:id="rId2"/>
     <sheet name="WAMI PRINCIPAL" sheetId="4" r:id="rId3"/>
-    <sheet name="principaldata" sheetId="5" r:id="rId4"/>
+    <sheet name="principaldata" sheetId="5" state="hidden" r:id="rId4"/>
     <sheet name="principalall" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="330">
-  <si>
-    <t>nelialopez</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="329">
   <si>
     <t>username</t>
   </si>
@@ -54,18 +51,9 @@
     <t>LOGOUT</t>
   </si>
   <si>
-    <t>nelia1234</t>
-  </si>
-  <si>
     <t>lastname</t>
   </si>
   <si>
-    <t>Nelia</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
     <t>mark1234</t>
   </si>
   <si>
@@ -1018,6 +1006,15 @@
   </si>
   <si>
     <t>LastName</t>
+  </si>
+  <si>
+    <t>vincelobina</t>
+  </si>
+  <si>
+    <t>Vince</t>
+  </si>
+  <si>
+    <t>Lobina</t>
   </si>
 </sst>
 </file>
@@ -1101,12 +1098,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G4:Y20"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:Y1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,134 +1397,134 @@
   </cols>
   <sheetData>
     <row r="4" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="4"/>
+      <c r="J4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="7"/>
       <c r="L4" s="1" t="str">
         <f>"INSERT INTO system_users_tbl SET user_name = '" &amp; $H$6&amp; "', password = '" &amp;$H$7 &amp;"', name = '" &amp; $H$8 &amp; "', last_name = '" &amp; $H$9 &amp;"' , account_type = 'User';"</f>
-        <v>INSERT INTO system_users_tbl SET user_name = 'nelialopez', password = 'nelia1234', name = 'Nelia', last_name = 'Lopez' , account_type = 'User';</v>
+        <v>INSERT INTO system_users_tbl SET user_name = 'vincelobina', password = 'vincelobina', name = 'Vince', last_name = 'Lobina' , account_type = 'User';</v>
       </c>
     </row>
     <row r="6" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="4"/>
+        <v>326</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="7"/>
       <c r="L6" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM KAS'; "</f>
-        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM KAS'; </v>
+        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM KAS'; </v>
       </c>
     </row>
     <row r="7" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+        <v>326</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM WHOLE SALER'; "</f>
-        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM WHOLE SALER'; </v>
+        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM WHOLE SALER'; </v>
       </c>
     </row>
     <row r="8" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+        <v>327</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM ARMAN'; "</f>
-        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM ARMAN'; </v>
+        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM ARMAN'; </v>
       </c>
     </row>
     <row r="9" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+        <v>328</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JR'; "</f>
-        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JR'; </v>
+        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JR'; </v>
       </c>
     </row>
     <row r="10" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JOMAR'; "</f>
-        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JOMAR'; </v>
+        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JOMAR'; </v>
       </c>
     </row>
     <row r="11" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM FRONERI'; "</f>
-        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM FRONERI'; </v>
+        <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM FRONERI'; </v>
       </c>
     </row>
     <row r="12" spans="7:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="7:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="4"/>
+      <c r="J14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="7"/>
       <c r="L14" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER TEAM';"</f>
-        <v>INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'MODULE_ACCESS', constant_value = 'PER TEAM';</v>
+        <v>INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'MODULE_ACCESS', constant_value = 'PER TEAM';</v>
       </c>
     </row>
     <row r="15" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER SALESMAN';"</f>
-        <v>INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'MODULE_ACCESS', constant_value = 'PER SALESMAN';</v>
+        <v>INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'MODULE_ACCESS', constant_value = 'PER SALESMAN';</v>
       </c>
     </row>
     <row r="16" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
       <c r="L16" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER PRINCIPAL';"</f>
-        <v>INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'MODULE_ACCESS', constant_value = 'PER PRINCIPAL';</v>
+        <v>INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'MODULE_ACCESS', constant_value = 'PER PRINCIPAL';</v>
       </c>
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
       <c r="L17" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER AREA';"</f>
-        <v>INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'MODULE_ACCESS', constant_value = 'PER AREA';</v>
+        <v>INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'MODULE_ACCESS', constant_value = 'PER AREA';</v>
       </c>
     </row>
     <row r="18" spans="10:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="4"/>
+      <c r="J20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="7"/>
       <c r="L20" s="1" t="str">
-        <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE"</f>
-        <v>INSERT INTO system_users_access SET user_name = 'nelialopez', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE</v>
+        <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE'"</f>
+        <v>INSERT INTO system_users_access SET user_name = 'vincelobina', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE'</v>
       </c>
     </row>
   </sheetData>
@@ -1557,10 +1554,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="4"/>
+      <c r="J4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="7"/>
       <c r="L4" s="1" t="str">
         <f>"INSERT INTO system_users_tbl SET user_name = '" &amp; $H$6&amp; "', password = '" &amp;$H$7 &amp;"', name = '" &amp; $H$8 &amp; "', last_name = '" &amp; $H$9 &amp;"' , account_type = 'User';"</f>
         <v>INSERT INTO system_users_tbl SET user_name = 'marksoliman', password = 'mark1234', name = 'Mark', last_name = 'Soliman' , account_type = 'User';</v>
@@ -1568,15 +1565,15 @@
     </row>
     <row r="6" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="7"/>
       <c r="L6" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM KAS'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM KAS'; </v>
@@ -1584,13 +1581,13 @@
     </row>
     <row r="7" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM WHOLE SALER'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM WHOLE SALER'; </v>
@@ -1598,13 +1595,13 @@
     </row>
     <row r="8" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM ARMAN'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM ARMAN'; </v>
@@ -1612,13 +1609,13 @@
     </row>
     <row r="9" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JR'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JR'; </v>
@@ -1626,21 +1623,21 @@
     </row>
     <row r="10" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G10" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JOMAR'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JOMAR'; </v>
       </c>
     </row>
     <row r="11" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM FRONERI'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM FRONERI'; </v>
@@ -1649,34 +1646,34 @@
     <row r="12" spans="7:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="7:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="4"/>
+      <c r="J14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="7"/>
       <c r="L14" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER TEAM';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'MODULE_ACCESS', constant_value = 'PER TEAM';</v>
       </c>
     </row>
     <row r="15" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER SALESMAN';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'MODULE_ACCESS', constant_value = 'PER SALESMAN';</v>
       </c>
     </row>
     <row r="16" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
       <c r="L16" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER PRINCIPAL';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'MODULE_ACCESS', constant_value = 'PER PRINCIPAL';</v>
       </c>
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
       <c r="L17" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER AREA';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'MODULE_ACCESS', constant_value = 'PER AREA';</v>
@@ -1684,20 +1681,20 @@
     </row>
     <row r="18" spans="10:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="4"/>
+      <c r="J20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="7"/>
       <c r="L20" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE';</v>
       </c>
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="4"/>
+      <c r="J22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="7"/>
       <c r="L22" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'SALES_POSITION_NAME', constant_value = '" &amp; $H$10 &amp; "';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'marksoliman', constant_type = 'SALES_POSITION_NAME', constant_value = 'SP11104901';</v>
@@ -1719,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G4:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20:Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,10 +1728,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="4"/>
+      <c r="J4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="7"/>
       <c r="L4" s="1" t="str">
         <f>"INSERT INTO system_users_tbl SET user_name = '" &amp; $H$6&amp; "', password = '" &amp;$H$7 &amp;"', name = '" &amp; $H$8 &amp; "', last_name = '" &amp; $H$9 &amp;"' , account_type = 'User';"</f>
         <v>INSERT INTO system_users_tbl SET user_name = 'victorserrano', password = 'mark1234', name = 'Victor', last_name = 'Serrano' , account_type = 'User';</v>
@@ -1742,15 +1739,15 @@
     </row>
     <row r="6" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>316</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="4"/>
+        <v>312</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="7"/>
       <c r="L6" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM KAS'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM KAS'; </v>
@@ -1758,13 +1755,13 @@
     </row>
     <row r="7" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM WHOLE SALER'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM WHOLE SALER'; </v>
@@ -1772,14 +1769,14 @@
     </row>
     <row r="8" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2" t="str">
         <f>VLOOKUP(H6,principaldata!A:E,4,FALSE)</f>
         <v>Victor</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM ARMAN'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM ARMAN'; </v>
@@ -1787,14 +1784,14 @@
     </row>
     <row r="9" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2" t="str">
         <f>VLOOKUP(H6,principaldata!A:E,5,FALSE)</f>
         <v>Serrano</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JR'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JR'; </v>
@@ -1802,22 +1799,22 @@
     </row>
     <row r="10" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H10" s="3" t="str">
         <f>VLOOKUP(H6,principaldata!A:B,2,FALSE)</f>
         <v>P53980-1804</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JOMAR'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM JOMAR'; </v>
       </c>
     </row>
     <row r="11" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM FRONERI'; "</f>
         <v xml:space="preserve">INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'TEAM_ACCESS', constant_value = 'TEAM FRONERI'; </v>
@@ -1826,34 +1823,34 @@
     <row r="12" spans="7:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="7:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="4"/>
+      <c r="J14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="7"/>
       <c r="L14" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER TEAM';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'MODULE_ACCESS', constant_value = 'PER TEAM';</v>
       </c>
     </row>
     <row r="15" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER SALESMAN';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'MODULE_ACCESS', constant_value = 'PER SALESMAN';</v>
       </c>
     </row>
     <row r="16" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
       <c r="L16" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER PRINCIPAL';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'MODULE_ACCESS', constant_value = 'PER PRINCIPAL';</v>
       </c>
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
       <c r="L17" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6&amp; "', constant_type = 'MODULE_ACCESS', constant_value = 'PER AREA';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'MODULE_ACCESS', constant_value = 'PER AREA';</v>
@@ -1861,20 +1858,20 @@
     </row>
     <row r="18" spans="10:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="4"/>
+      <c r="J20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="7"/>
       <c r="L20" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'AUTO_LOGOUT', constant_value = 'FALSE';</v>
       </c>
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" s="4"/>
+      <c r="J22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="7"/>
       <c r="L22" s="1" t="str">
         <f>"INSERT INTO system_users_access SET user_name = '" &amp; $H$6 &amp; "', constant_type = 'PRINCIPAL_ACCESS', constant_value = '" &amp; $H$10 &amp; "';"</f>
         <v>INSERT INTO system_users_access SET user_name = 'victorserrano', constant_type = 'PRINCIPAL_ACCESS', constant_value = 'P53980-1804';</v>
@@ -1910,462 +1907,462 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>329</v>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E13" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E14" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E15" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E16" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B17" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E17" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B18" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E18" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B19" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E19" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B20" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E20" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E21" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B22" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E22" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B23" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E23" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B24" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E24" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B25" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E25" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B26" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E26" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B27" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E27" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2385,1092 +2382,1092 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>22</v>
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B43" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C46" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B53" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B54" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B55" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B57" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B58" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C59" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B60" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C60" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B61" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C61" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B62" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C63" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B65" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B66" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C66" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B67" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B68" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B69" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C69" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B70" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B72" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C72" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C73" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C74" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B75" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C75" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C76" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B77" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C77" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B79" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C79" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C80" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B81" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C81" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B82" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C82" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B83" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C83" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B84" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C84" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B85" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C85" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B86" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C86" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B87" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C87" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B88" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C88" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B89" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B90" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C90" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B91" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C91" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B92" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C92" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B93" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C93" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B94" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C94" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B95" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C95" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B96" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C96" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B97" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C97" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B98" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C98" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B99" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C99" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>